<commit_message>
fixed bug - bowlpool basic styles working
</commit_message>
<xml_diff>
--- a/backend/src/resources/bowlpool.xlsx
+++ b/backend/src/resources/bowlpool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanKennedy/Code/GitHub/bowlpoolReact/backend/src/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\CS 5319\CS-5319-Bowlpool\backend\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D22868-C9B8-A746-949B-0107AB6824F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55412D46-7157-462B-ABB7-9F37E1065E5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="140">
   <si>
     <t>Liberty</t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>Home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home </t>
   </si>
   <si>
     <t>MSK</t>
@@ -1745,26 +1742,26 @@
   <dimension ref="A1:AA80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="76"/>
-    <col min="2" max="2" width="14.6640625"/>
-    <col min="3" max="3" width="19.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" style="76"/>
+    <col min="2" max="2" width="14.625"/>
+    <col min="3" max="3" width="19.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="59" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" style="68" customWidth="1"/>
-    <col min="7" max="8" width="4.6640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="4.6640625" style="68" customWidth="1"/>
-    <col min="11" max="14" width="4.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" style="68" customWidth="1"/>
-    <col min="16" max="17" width="4.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" style="74" customWidth="1"/>
-    <col min="19" max="19" width="4.6640625" style="68" customWidth="1"/>
-    <col min="20" max="25" width="4.6640625" style="1" customWidth="1"/>
-    <col min="26" max="27" width="5.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.625" style="68" customWidth="1"/>
+    <col min="7" max="8" width="4.625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="4.625" style="68" customWidth="1"/>
+    <col min="11" max="14" width="4.625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4.625" style="68" customWidth="1"/>
+    <col min="16" max="17" width="4.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="4.625" style="74" customWidth="1"/>
+    <col min="19" max="19" width="4.625" style="68" customWidth="1"/>
+    <col min="20" max="25" width="4.625" style="1" customWidth="1"/>
+    <col min="26" max="27" width="5.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1">
@@ -1772,16 +1769,16 @@
         <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F1" s="61" t="s">
         <v>117</v>
@@ -1805,7 +1802,7 @@
         <v>122</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>124</v>
@@ -1817,7 +1814,7 @@
         <v>126</v>
       </c>
       <c r="Q1" s="117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R1" s="21" t="s">
         <v>127</v>
@@ -2086,7 +2083,7 @@
         <v>401135263</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>8</v>
@@ -2187,7 +2184,7 @@
       <c r="Z8" s="2"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" ht="16" customHeight="1" thickBot="1">
+    <row r="9" spans="1:27" ht="15.95" customHeight="1" thickBot="1">
       <c r="A9" s="77">
         <v>401147693</v>
       </c>
@@ -3319,7 +3316,7 @@
         <v>131</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>83</v>
@@ -4833,7 +4830,7 @@
         <v>131</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>83</v>
@@ -5778,7 +5775,7 @@
       <c r="X79" s="46"/>
       <c r="Y79" s="46"/>
     </row>
-    <row r="80" spans="1:27" ht="14" customHeight="1" thickTop="1">
+    <row r="80" spans="1:27" ht="14.1" customHeight="1" thickTop="1">
       <c r="G80" s="108"/>
       <c r="H80" s="108"/>
       <c r="I80" s="109"/>

</xml_diff>